<commit_message>
commit modications done on df_mini: remove duplicates
</commit_message>
<xml_diff>
--- a/dataframe_each_make_xlsx_file/df_mini_updated.xlsx
+++ b/dataframe_each_make_xlsx_file/df_mini_updated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,7 +782,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Clubman</t>
+          <t>Cooper (s) Hardtop &amp; Cabrio</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -810,7 +810,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Cooper (s) Hardtop &amp; Cabrio</t>
+          <t>Countryman</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -838,7 +838,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Countryman</t>
+          <t>Coupe</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Coupe</t>
+          <t>John Cooper Works</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -885,7 +885,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -894,7 +894,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>John Cooper Works</t>
+          <t>Clubman</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -904,7 +904,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>EWS III</t>
+          <t>Information not available</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Clubman</t>
+          <t>Cooper (s) Hardtop &amp; Cabrio</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Clubman</t>
+          <t>Countryman</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -978,7 +978,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Cooper (s) Hardtop &amp; Cabrio</t>
+          <t>Coupe</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Countryman</t>
+          <t>John Cooper Works</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1015,62 +1015,6 @@
         </is>
       </c>
       <c r="F21" t="inlineStr">
-        <is>
-          <t>Information not available</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Mini</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Coupe</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Std</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Information not available</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Mini</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>John Cooper Works</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Std</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
         <is>
           <t>Information not available</t>
         </is>

</xml_diff>